<commit_message>
updated boms in excel
</commit_message>
<xml_diff>
--- a/hardware/impulse/rev_a/impulse_bom.xlsx
+++ b/hardware/impulse/rev_a/impulse_bom.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="16100" tabRatio="114"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -305,7 +309,7 @@
     <t>FM25L04B-DGRA-ND</t>
   </si>
   <si>
-    <t> 877-FM25L04B-DG </t>
+    <t>877-FM25L04B-DG</t>
   </si>
   <si>
     <t>MSP430F1611IRTD</t>
@@ -347,41 +351,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
       <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,100 +384,386 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="hair"/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="30.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.9183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8316326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col min="2" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,610 +792,614 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:9">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:9">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:9">
+      <c r="A8">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
-      <c r="A11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="0" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="C16" s="0" t="s">
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="n">
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
         <v>470</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="A18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" s="0" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="A19" s="0" t="n">
+    <row r="19" spans="1:8">
+      <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="0" t="s">
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
-      <c r="A21" s="0" t="n">
+    <row r="21" spans="1:8">
+      <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
-      <c r="A22" s="0" t="n">
+    <row r="22" spans="1:8">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
-      <c r="A23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" s="0" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
-      <c r="A24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B24" s="0" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
-      <c r="A25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" s="0" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="G25" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
-      <c r="A26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="0" t="s">
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="G26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B27" s="0" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" t="s">
         <v>103</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" t="s">
         <v>104</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" t="s">
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="G28" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05416666666667" bottom="0.7875" header="0.7875" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="38" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.79" right="0.79" top="1.05" bottom="0.79" header="0.79" footer="0.51"/>
+  <pageSetup scale="56" orientation="landscape" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter/>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>